<commit_message>
anonymised company name, client manager name from test files
</commit_message>
<xml_diff>
--- a/src/main/resources/test file 2.xlsx
+++ b/src/main/resources/test file 2.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Filter:</t>
   </si>
   <si>
-    <t xml:space="preserve">Vendor/Company Name = 'SECURITAS' AND First Name Is Not Blank AND Last Name Is Not Blank AND Contractor/Vendor Number Begins With 'STUART BRACE' AND Event Date &gt;= '20210524 4:19:34 AM' AND Event Date &lt;= '20210525 12:19:34 PM'</t>
+    <t xml:space="preserve">Vendor/Company Name = 'COMPANY NAME' AND First Name Is Not Blank AND Last Name Is Not Blank AND Contractor/Vendor Number Begins With 'CLIENT MANAGER' AND Event Date &gt;= '20210524 4:19:34 AM' AND Event Date &lt;= '20210525 12:19:34 PM'</t>
   </si>
   <si>
     <t xml:space="preserve">Report Date:</t>
@@ -82,10 +82,13 @@
     <t xml:space="preserve">Contractor </t>
   </si>
   <si>
+    <t xml:space="preserve">Company Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">PLA0101 - Barrier IN</t>
   </si>
   <si>
-    <t xml:space="preserve">Securitas - S Brace</t>
+    <t xml:space="preserve">Comp Name – C Mgr</t>
   </si>
   <si>
     <t xml:space="preserve">Stuart Brace</t>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">officer 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECURITAS</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0901 - Turnstile South IN</t>
@@ -438,11 +438,11 @@
   </sheetPr>
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F117" activeCellId="0" sqref="F117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -519,7 +519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -533,19 +533,19 @@
         <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -558,20 +558,20 @@
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>1</v>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -585,19 +585,19 @@
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -611,19 +611,19 @@
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -637,19 +637,19 @@
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -663,19 +663,19 @@
         <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -689,19 +689,19 @@
         <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -715,19 +715,19 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -740,25 +740,25 @@
       <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>1</v>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>44340.2440856481</v>
@@ -767,24 +767,24 @@
         <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>44340.2499768519</v>
@@ -792,25 +792,25 @@
       <c r="D18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>28</v>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>21</v>
+      <c r="G18" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>44340.7377083333</v>
@@ -819,24 +819,24 @@
         <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>44340.7465393519</v>
@@ -845,24 +845,24 @@
         <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>44340.7609490741</v>
@@ -870,20 +870,20 @@
       <c r="D21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>28</v>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>21</v>
+      <c r="G21" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -897,19 +897,19 @@
         <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
@@ -922,20 +922,20 @@
       <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>1</v>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
@@ -949,19 +949,19 @@
         <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -975,19 +975,19 @@
         <v>19</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1001,13 +1001,13 @@
         <v>19</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>30</v>
@@ -1026,14 +1026,14 @@
       <c r="D27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>28</v>
+      <c r="E27" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>21</v>
+      <c r="G27" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>30</v>
@@ -1052,20 +1052,20 @@
       <c r="D28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>28</v>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>21</v>
+      <c r="G28" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -1079,19 +1079,19 @@
         <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -1105,19 +1105,19 @@
         <v>19</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
@@ -1131,19 +1131,19 @@
         <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1157,19 +1157,19 @@
         <v>19</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -1183,19 +1183,19 @@
         <v>19</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1209,19 +1209,19 @@
         <v>19</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>37</v>
       </c>
@@ -1235,19 +1235,19 @@
         <v>19</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1261,19 +1261,19 @@
         <v>19</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>37</v>
       </c>
@@ -1286,20 +1286,20 @@
       <c r="D37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>1</v>
+      <c r="E37" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>21</v>
+      <c r="G37" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1313,19 +1313,19 @@
         <v>19</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1339,19 +1339,19 @@
         <v>19</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
@@ -1365,19 +1365,19 @@
         <v>19</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -1391,19 +1391,19 @@
         <v>19</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -1417,19 +1417,19 @@
         <v>19</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>37</v>
       </c>
@@ -1443,19 +1443,19 @@
         <v>19</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>37</v>
       </c>
@@ -1469,19 +1469,19 @@
         <v>19</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>37</v>
       </c>
@@ -1495,19 +1495,19 @@
         <v>19</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
@@ -1521,19 +1521,19 @@
         <v>19</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>37</v>
       </c>
@@ -1547,19 +1547,19 @@
         <v>19</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>37</v>
       </c>
@@ -1573,19 +1573,19 @@
         <v>19</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>37</v>
       </c>
@@ -1599,19 +1599,19 @@
         <v>19</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>37</v>
       </c>
@@ -1625,19 +1625,19 @@
         <v>19</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>37</v>
       </c>
@@ -1651,19 +1651,19 @@
         <v>19</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>37</v>
       </c>
@@ -1677,19 +1677,19 @@
         <v>19</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>37</v>
       </c>
@@ -1703,19 +1703,19 @@
         <v>19</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>37</v>
       </c>
@@ -1729,19 +1729,19 @@
         <v>19</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>37</v>
       </c>
@@ -1755,19 +1755,19 @@
         <v>19</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>37</v>
       </c>
@@ -1781,19 +1781,19 @@
         <v>19</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>37</v>
       </c>
@@ -1807,19 +1807,19 @@
         <v>19</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -1833,19 +1833,19 @@
         <v>19</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>37</v>
       </c>
@@ -1859,19 +1859,19 @@
         <v>19</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -1885,19 +1885,19 @@
         <v>19</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -1911,19 +1911,19 @@
         <v>19</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
         <v>37</v>
       </c>
@@ -1937,19 +1937,19 @@
         <v>19</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>37</v>
       </c>
@@ -1963,19 +1963,19 @@
         <v>19</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
         <v>37</v>
       </c>
@@ -1989,19 +1989,19 @@
         <v>19</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>37</v>
       </c>
@@ -2015,19 +2015,19 @@
         <v>19</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
         <v>37</v>
       </c>
@@ -2041,19 +2041,19 @@
         <v>19</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>37</v>
       </c>
@@ -2067,19 +2067,19 @@
         <v>19</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>37</v>
       </c>
@@ -2093,19 +2093,19 @@
         <v>19</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>37</v>
       </c>
@@ -2119,19 +2119,19 @@
         <v>19</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="70" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>37</v>
       </c>
@@ -2144,17 +2144,17 @@
       <c r="D70" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>1</v>
+      <c r="E70" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G70" s="5" t="s">
-        <v>21</v>
+      <c r="G70" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,17 +2170,17 @@
       <c r="D71" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>1</v>
+      <c r="E71" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G71" s="5" t="s">
-        <v>21</v>
+      <c r="G71" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,20 +2196,20 @@
       <c r="D72" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>1</v>
+      <c r="E72" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G72" s="5" t="s">
-        <v>21</v>
+      <c r="G72" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -2223,19 +2223,19 @@
         <v>19</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>56</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -2249,19 +2249,19 @@
         <v>19</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
         <v>58</v>
       </c>
@@ -2275,19 +2275,19 @@
         <v>19</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="76" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>58</v>
       </c>
@@ -2300,20 +2300,20 @@
       <c r="D76" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>1</v>
+      <c r="E76" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G76" s="5" t="s">
-        <v>21</v>
+      <c r="G76" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="77" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>58</v>
       </c>
@@ -2326,20 +2326,20 @@
       <c r="D77" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>1</v>
+      <c r="E77" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G77" s="5" t="s">
-        <v>21</v>
+      <c r="G77" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
         <v>58</v>
       </c>
@@ -2353,19 +2353,19 @@
         <v>19</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
         <v>58</v>
       </c>
@@ -2379,19 +2379,19 @@
         <v>19</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
         <v>58</v>
       </c>
@@ -2405,19 +2405,19 @@
         <v>19</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>55</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
         <v>59</v>
       </c>
@@ -2431,19 +2431,19 @@
         <v>19</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>59</v>
       </c>
@@ -2456,20 +2456,20 @@
       <c r="D82" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E82" s="5" t="s">
-        <v>1</v>
+      <c r="E82" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G82" s="5" t="s">
-        <v>21</v>
+      <c r="G82" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
         <v>59</v>
       </c>
@@ -2483,19 +2483,19 @@
         <v>19</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>59</v>
       </c>
@@ -2509,19 +2509,19 @@
         <v>19</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
         <v>59</v>
       </c>
@@ -2535,19 +2535,19 @@
         <v>19</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
         <v>59</v>
       </c>
@@ -2561,19 +2561,19 @@
         <v>19</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
         <v>59</v>
       </c>
@@ -2587,19 +2587,19 @@
         <v>19</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
         <v>59</v>
       </c>
@@ -2613,19 +2613,19 @@
         <v>19</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
         <v>59</v>
       </c>
@@ -2639,19 +2639,19 @@
         <v>19</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
         <v>59</v>
       </c>
@@ -2665,19 +2665,19 @@
         <v>19</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
         <v>59</v>
       </c>
@@ -2691,16 +2691,16 @@
         <v>19</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,20 +2716,20 @@
       <c r="D92" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E92" s="5" t="s">
-        <v>1</v>
+      <c r="E92" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G92" s="5" t="s">
-        <v>21</v>
+      <c r="G92" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
         <v>59</v>
       </c>
@@ -2743,19 +2743,19 @@
         <v>19</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
         <v>59</v>
       </c>
@@ -2769,19 +2769,19 @@
         <v>19</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
         <v>59</v>
       </c>
@@ -2795,19 +2795,19 @@
         <v>19</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
         <v>59</v>
       </c>
@@ -2821,19 +2821,19 @@
         <v>19</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
         <v>59</v>
       </c>
@@ -2847,19 +2847,19 @@
         <v>19</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>59</v>
       </c>
@@ -2873,19 +2873,19 @@
         <v>19</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>59</v>
       </c>
@@ -2899,19 +2899,19 @@
         <v>19</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="100" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
         <v>61</v>
       </c>
@@ -2924,20 +2924,20 @@
       <c r="D100" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>1</v>
+      <c r="E100" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G100" s="5" t="s">
-        <v>21</v>
+      <c r="G100" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>61</v>
       </c>
@@ -2951,19 +2951,19 @@
         <v>19</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>61</v>
       </c>
@@ -2977,19 +2977,19 @@
         <v>19</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>61</v>
       </c>
@@ -3003,19 +3003,19 @@
         <v>19</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>61</v>
       </c>
@@ -3029,19 +3029,19 @@
         <v>19</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>61</v>
       </c>
@@ -3055,19 +3055,19 @@
         <v>19</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>61</v>
       </c>
@@ -3081,19 +3081,19 @@
         <v>19</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>61</v>
       </c>
@@ -3107,19 +3107,19 @@
         <v>19</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>61</v>
       </c>
@@ -3133,19 +3133,19 @@
         <v>19</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>61</v>
       </c>
@@ -3159,19 +3159,19 @@
         <v>19</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
         <v>61</v>
       </c>
@@ -3185,19 +3185,19 @@
         <v>19</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
         <v>61</v>
       </c>
@@ -3211,19 +3211,19 @@
         <v>19</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
         <v>61</v>
       </c>
@@ -3237,19 +3237,19 @@
         <v>19</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
         <v>61</v>
       </c>
@@ -3263,19 +3263,19 @@
         <v>19</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>61</v>
       </c>
@@ -3289,19 +3289,19 @@
         <v>19</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>61</v>
       </c>
@@ -3315,19 +3315,19 @@
         <v>19</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
         <v>61</v>
       </c>
@@ -3341,19 +3341,19 @@
         <v>19</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F116" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>61</v>
       </c>
@@ -3367,19 +3367,19 @@
         <v>19</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>61</v>
       </c>
@@ -3393,19 +3393,19 @@
         <v>19</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
         <v>61</v>
       </c>
@@ -3419,19 +3419,19 @@
         <v>19</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>61</v>
       </c>
@@ -3445,19 +3445,19 @@
         <v>19</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
         <v>61</v>
       </c>
@@ -3471,19 +3471,19 @@
         <v>19</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F121" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
         <v>61</v>
       </c>
@@ -3497,19 +3497,19 @@
         <v>19</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F122" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="123" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
         <v>61</v>
       </c>
@@ -3522,20 +3522,20 @@
       <c r="D123" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E123" s="5" t="s">
-        <v>1</v>
+      <c r="E123" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G123" s="5" t="s">
-        <v>21</v>
+      <c r="G123" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
         <v>61</v>
       </c>
@@ -3549,19 +3549,19 @@
         <v>19</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F124" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
         <v>61</v>
       </c>
@@ -3575,19 +3575,19 @@
         <v>19</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>61</v>
       </c>
@@ -3601,19 +3601,19 @@
         <v>19</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
         <v>61</v>
       </c>
@@ -3627,19 +3627,19 @@
         <v>19</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
         <v>61</v>
       </c>
@@ -3653,19 +3653,19 @@
         <v>19</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
         <v>61</v>
       </c>
@@ -3679,19 +3679,19 @@
         <v>19</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F129" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
         <v>61</v>
       </c>
@@ -3705,19 +3705,19 @@
         <v>19</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
         <v>61</v>
       </c>
@@ -3731,19 +3731,19 @@
         <v>19</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
         <v>61</v>
       </c>
@@ -3757,19 +3757,19 @@
         <v>19</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
         <v>61</v>
       </c>
@@ -3783,19 +3783,19 @@
         <v>19</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
         <v>61</v>
       </c>
@@ -3809,19 +3809,19 @@
         <v>19</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
         <v>61</v>
       </c>
@@ -3835,19 +3835,19 @@
         <v>19</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F135" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
         <v>61</v>
       </c>
@@ -3861,19 +3861,19 @@
         <v>19</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F136" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
         <v>61</v>
       </c>
@@ -3887,19 +3887,19 @@
         <v>19</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F137" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
         <v>61</v>
       </c>
@@ -3913,19 +3913,19 @@
         <v>19</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
         <v>61</v>
       </c>
@@ -3939,19 +3939,19 @@
         <v>19</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
         <v>61</v>
       </c>
@@ -3965,19 +3965,19 @@
         <v>19</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F140" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
         <v>61</v>
       </c>
@@ -3991,19 +3991,19 @@
         <v>19</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F141" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
         <v>61</v>
       </c>
@@ -4017,19 +4017,19 @@
         <v>19</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F142" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>61</v>
       </c>
@@ -4043,19 +4043,19 @@
         <v>19</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F143" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>61</v>
       </c>
@@ -4069,16 +4069,16 @@
         <v>19</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F144" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Already anonymised, For better looking sample run now first Name of all officer is 'officer' and last name is 'One', 'Two' and so on
</commit_message>
<xml_diff>
--- a/src/main/resources/test file 2.xlsx
+++ b/src/main/resources/test file 2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="64">
   <si>
     <t xml:space="preserve">Report Title:</t>
   </si>
@@ -76,7 +76,10 @@
     <t xml:space="preserve">Contractor/Vendor Number</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 1</t>
+    <t xml:space="preserve">Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One</t>
   </si>
   <si>
     <t xml:space="preserve">Contractor </t>
@@ -103,10 +106,10 @@
     <t xml:space="preserve">PLA0103 - Turnstile West OUT</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officer 3</t>
+    <t xml:space="preserve">Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0901 - Turnstile South IN</t>
@@ -121,19 +124,19 @@
     <t xml:space="preserve">Thames LSI0904 - Turnstile North OUT</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officer 5</t>
+    <t xml:space="preserve">Four</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Five</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0903 - Turnstile North IN</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officer 7</t>
+    <t xml:space="preserve">Six</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seven</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0604 - 2nd Floor West</t>
@@ -184,7 +187,7 @@
     <t xml:space="preserve">Thames LSI0308 - Empl Cr Pk Barrier OUT</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 8</t>
+    <t xml:space="preserve">Eight</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0701 - Weighbridge IN</t>
@@ -193,19 +196,19 @@
     <t xml:space="preserve">Thames LSI0702 - Weighbridge OUT</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officer 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officer 11</t>
+    <t xml:space="preserve">Nine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eleven</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI1201 - TIE Turnstile IN</t>
   </si>
   <si>
-    <t xml:space="preserve">officer 12</t>
+    <t xml:space="preserve">Twelve</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0502 - HR Office West</t>
@@ -347,11 +350,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,11 +441,11 @@
   </sheetPr>
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A126" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D139" activeCellId="0" sqref="D139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -524,51 +527,51 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>44340.7379282407</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="5" t="n">
         <v>44340.7391203704</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
+      <c r="D9" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,25 +579,25 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>44340.8389699074</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,25 +605,25 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>44340.8458680556</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,25 +631,25 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>44340.8514583333</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,25 +657,25 @@
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>44341.0562615741</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,25 +683,25 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>44341.063125</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,3379 +709,3379 @@
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>44341.0685300926</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="5" t="n">
         <v>44341.2429166667</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
+      <c r="D16" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>44340.2440856481</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="6" t="n">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="n">
         <v>44340.2499768519</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
+      <c r="D18" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>44340.7377083333</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>44340.7465393519</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="21" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="6" t="n">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="5" t="n">
         <v>44340.7609490741</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>19</v>
+      <c r="D21" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>44340.3540740741</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="6" t="n">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="5" t="n">
         <v>44340.7474884259</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
+      <c r="D23" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>44341.2378356481</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>44341.2488078704</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>44340.2513888889</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>44340.7410532407</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="6" t="n">
-        <v>44340.7410532407</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="G27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="6" t="n">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5" t="n">
         <v>44341.2530208333</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>19</v>
+      <c r="D28" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>44340.1806018519</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>44340.1825462963</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>44340.1841782407</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>44340.2278935185</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>44340.2284606481</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>44340.228900463</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>44340.2355324074</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>44340.742974537</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="6" t="n">
+      <c r="A37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="5" t="n">
         <v>44340.7448726852</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>19</v>
+      <c r="D37" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>44340.8461805556</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>44340.8562615741</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>44340.8576967593</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>44340.8581944444</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>44340.8593634259</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>44340.8599652778</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>44340.8649884259</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>44340.8669212963</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>44340.8697106481</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>44340.9333217593</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>44340.9350578704</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>44340.9377430556</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>44340.9416203704</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>44340.9470486111</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>44341.0060300926</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>44341.1601736111</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>44341.1646643519</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>44341.1746064815</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>44341.1790393519</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>44341.1795717593</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>44341.1800578704</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>44341.1819097222</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>44341.1820949074</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>44341.1841087963</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>44341.1841782407</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>44341.1847453704</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>44341.1876388889</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>44341.1895601852</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>44341.1910532407</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>44341.2286574074</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>44341.2290856481</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>44341.2296527778</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" s="6" t="n">
+      <c r="A70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="5" t="n">
         <v>44341.2411921296</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>19</v>
+      <c r="D70" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="71" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C71" s="6" t="n">
+      <c r="A71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="5" t="n">
         <v>44340.743912037</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>19</v>
+      <c r="D71" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F71" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C72" s="6" t="n">
+      <c r="C72" s="5" t="n">
         <v>44341.2467013889</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>19</v>
+      <c r="D72" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>44340.2538773148</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C74" s="4" t="n">
         <v>44340.2583333333</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>44340.2469444444</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C76" s="6" t="n">
+      <c r="A76" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="5" t="n">
         <v>44340.2522916667</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>19</v>
+      <c r="D76" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="77" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C77" s="6" t="n">
+      <c r="A77" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" s="5" t="n">
         <v>44340.746087963</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>19</v>
+      <c r="D77" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C78" s="4" t="n">
         <v>44340.7510648148</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>44341.2448842593</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C80" s="4" t="n">
         <v>44341.2466319444</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>44340.227337963</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F81" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="82" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="6" t="n">
+      <c r="C82" s="5" t="n">
         <v>44340.2287384259</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>19</v>
+      <c r="D82" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C83" s="4" t="n">
         <v>44340.2541782407</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>44340.2547222222</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C85" s="4" t="n">
         <v>44340.2559027778</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>44340.2564236111</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C87" s="4" t="n">
         <v>44340.2848726852</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>44340.5283101852</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>44340.5284837963</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C90" s="4" t="n">
         <v>44340.5821643519</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C91" s="4" t="n">
         <v>44340.5855439815</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C92" s="6" t="n">
+      <c r="A92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" s="5" t="n">
         <v>44340.7448958333</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>19</v>
+      <c r="D92" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>44341.2390393519</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>44341.2404166667</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C95" s="4" t="n">
         <v>44341.2518981481</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C96" s="4" t="n">
         <v>44341.2525694444</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>44341.2537615741</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C98" s="4" t="n">
         <v>44341.2543981482</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C99" s="4" t="n">
         <v>44341.2544560185</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C100" s="6" t="n">
+      <c r="A100" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" s="5" t="n">
         <v>44340.2827662037</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>19</v>
+      <c r="D100" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>44340.2830324074</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C102" s="4" t="n">
         <v>44340.2855555556</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C103" s="4" t="n">
         <v>44340.2877430556</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C104" s="4" t="n">
         <v>44340.2890856481</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C105" s="4" t="n">
         <v>44340.2913194444</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C106" s="4" t="n">
         <v>44340.2935069444</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>44340.3058217593</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C108" s="4" t="n">
         <v>44340.3062268519</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C109" s="4" t="n">
         <v>44340.3500578704</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C110" s="4" t="n">
         <v>44340.3508333333</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C111" s="4" t="n">
         <v>44340.3755671296</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C112" s="4" t="n">
         <v>44340.3757291667</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C113" s="4" t="n">
         <v>44340.3852662037</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>44340.6082175926</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C115" s="4" t="n">
         <v>44340.6083680556</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C116" s="4" t="n">
         <v>44340.6464930556</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>44340.6560185185</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>44340.685775463</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C119" s="4" t="n">
         <v>44340.6859490741</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C120" s="4" t="n">
         <v>44340.7027893519</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>44340.702974537</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C122" s="4" t="n">
         <v>44340.7300231481</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C123" s="6" t="n">
+      <c r="A123" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C123" s="5" t="n">
         <v>44340.7302430556</v>
       </c>
-      <c r="D123" s="5" t="s">
-        <v>19</v>
+      <c r="D123" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H123" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C124" s="4" t="n">
         <v>44341.2839814815</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>44341.2843171296</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>44341.2864930556</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C127" s="4" t="n">
         <v>44341.2892708333</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C128" s="4" t="n">
         <v>44341.2907407407</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C129" s="4" t="n">
         <v>44341.2928472222</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>44341.2950231481</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C131" s="4" t="n">
         <v>44341.3069675926</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C132" s="4" t="n">
         <v>44341.3071412037</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C133" s="4" t="n">
         <v>44341.3298842593</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C134" s="4" t="n">
         <v>44341.3299884259</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C135" s="4" t="n">
         <v>44341.3597337963</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C136" s="4" t="n">
         <v>44341.3829976852</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>44341.3831712963</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C138" s="4" t="n">
         <v>44341.3919560185</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C139" s="4" t="n">
         <v>44341.4045138889</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C140" s="4" t="n">
         <v>44341.4271180556</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C141" s="4" t="n">
         <v>44341.4272800926</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C142" s="4" t="n">
         <v>44341.4275462963</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>44341.4277546296</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C144" s="4" t="n">
         <v>44341.4364236111</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>